<commit_message>
changes for MVC structure of project
</commit_message>
<xml_diff>
--- a/core/sample_file/rosters/sample_roster.xlsx
+++ b/core/sample_file/rosters/sample_roster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bdmyers/rubricapp/rubricapp/sample_file/rosters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sahammond/rubricapp/core/sample_file/rosters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6099A8-A8B0-E540-B596-E9DDB427EDB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B787C5DB-4D93-4B4E-AD32-906235A40B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="1900" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="3500" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -330,17 +330,20 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -668,13 +671,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>